<commit_message>
Mise à jour des json pour dr plante
</commit_message>
<xml_diff>
--- a/csv/dr_plante.xlsx
+++ b/csv/dr_plante.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adl\Documents\Personnel\mon_jardin\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA90DEC3-429E-4829-A5F1-6DBE33769113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD86AD2C-1D2E-40BC-AAB5-A480011ABE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7B00D0DC-6EAF-4CB2-B2A7-8C532840F16C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{7B00D0DC-6EAF-4CB2-B2A7-8C532840F16C}"/>
   </bookViews>
   <sheets>
     <sheet name="Apparence feuilles" sheetId="1" r:id="rId1"/>
@@ -1842,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70C1E80-1A00-455A-AB30-ACEF23F0CEB6}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,7 +1946,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2076,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9265A2DD-438D-4402-875F-6BC5807A1A00}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>